<commit_message>
RSD Retrofit: Use LimType FX with NCAP_AF
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
+++ b/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6353FC-86BA-43D3-81CE-F6963F981C42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB835FD9-6C84-4226-878B-20ED424AD4D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSlices" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="66">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>S*</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -382,11 +388,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:G3" totalsRowShown="0">
-  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H3" totalsRowShown="0">
+  <autoFilter ref="B2:H3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
+    <tableColumn id="7" xr3:uid="{DA5FA9F4-D4B7-44E0-A803-2D2586DBF9CB}" name="LimType"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
@@ -778,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1308,18 +1315,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:G3"/>
+  <dimension ref="B1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1327,35 +1336,41 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3">
         <v>2018</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
     </row>

</xml_diff>